<commit_message>
add otp and modal components
</commit_message>
<xml_diff>
--- a/decentralized-voting-system/server/config/random_emails_aadhaar_1000.xlsx
+++ b/decentralized-voting-system/server/config/random_emails_aadhaar_1000.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1003"/>
+  <dimension ref="A1:D1004"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -14431,6 +14431,12 @@
       </c>
     </row>
     <row r="1003">
+      <c r="A1003" t="str">
+        <v/>
+      </c>
+      <c r="B1003" t="str">
+        <v/>
+      </c>
       <c r="C1003" t="str">
         <v>797971326062</v>
       </c>
@@ -14438,9 +14444,17 @@
         <v>shreemanthkunthe6@gmail.com</v>
       </c>
     </row>
+    <row r="1004">
+      <c r="C1004" t="str">
+        <v>797971326000</v>
+      </c>
+      <c r="D1004" t="str">
+        <v>anir52822@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D1003"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D1004"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjustments to mobile view
</commit_message>
<xml_diff>
--- a/decentralized-voting-system/server/config/random_emails_aadhaar_1000.xlsx
+++ b/decentralized-voting-system/server/config/random_emails_aadhaar_1000.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D1004"/>
+  <dimension ref="A1:D1005"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -14445,6 +14445,12 @@
       </c>
     </row>
     <row r="1004">
+      <c r="A1004" t="str">
+        <v/>
+      </c>
+      <c r="B1004" t="str">
+        <v/>
+      </c>
       <c r="C1004" t="str">
         <v>797971326000</v>
       </c>
@@ -14452,9 +14458,17 @@
         <v>anir52822@gmail.com</v>
       </c>
     </row>
+    <row r="1005">
+      <c r="C1005" t="str">
+        <v>797971326008</v>
+      </c>
+      <c r="D1005" t="str">
+        <v>a30488782@gmail.com</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D1004"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D1005"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>